<commit_message>
Fix BAU vehicle price in BESP
</commit_message>
<xml_diff>
--- a/InputData/trans/BESP/BAU EV Subsidy Perc.xlsx
+++ b/InputData/trans/BESP/BAU EV Subsidy Perc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-oregon\InputData\trans\BESP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E268DCE8-82CA-4342-ADA7-1C54E4F4A1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1A0301-44E7-4011-AF8B-05BA3D3022C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId8"/>
+    <pivotCache cacheId="41" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -573,7 +573,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -603,6 +603,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -1628,133 +1629,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable4" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A22:B41" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="23">
-        <item x="10"/>
-        <item x="5"/>
-        <item m="1" x="21"/>
-        <item x="16"/>
-        <item m="1" x="19"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="15"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item x="13"/>
-        <item m="1" x="20"/>
-        <item x="11"/>
-        <item x="4"/>
-        <item x="12"/>
-        <item m="1" x="18"/>
-        <item x="17"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="14"/>
-        <item x="8"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="19">
-    <i/>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i t="grand"/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of TOTAL" fld="15" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable5" cacheId="41" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G22:J40" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField axis="axisRow" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -1966,6 +1841,132 @@
     <dataField name="Sum of JAN" fld="3" baseField="0" baseItem="0"/>
     <dataField name="Sum of FEB" fld="4" baseField="0" baseItem="0"/>
     <dataField name="Sum of MAR" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable4" cacheId="41" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A22:B41" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="23">
+        <item x="10"/>
+        <item x="5"/>
+        <item m="1" x="21"/>
+        <item x="16"/>
+        <item m="1" x="19"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="15"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="13"/>
+        <item m="1" x="20"/>
+        <item x="11"/>
+        <item x="4"/>
+        <item x="12"/>
+        <item m="1" x="18"/>
+        <item x="17"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="14"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="19">
+    <i/>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i t="grand"/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of TOTAL" fld="15" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -2472,10 +2473,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AH30"/>
+  <dimension ref="A1:AG92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:AF11"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2485,12 +2486,12 @@
     <col min="3" max="3" width="19.1796875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -2588,7 +2589,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="12">
         <f>BAU!C92</f>
         <v>2745.8606136031594</v>
@@ -2718,31 +2719,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="12"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="12"/>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>2500</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" s="12"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10"/>
       <c r="B10">
         <v>2020</v>
@@ -2838,7 +2839,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" s="12"/>
       <c r="B11" s="12">
         <f>(B3+$A$7)*About!$B$34</f>
@@ -2965,7 +2966,7 @@
         <v>2217.7766787346754</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -3063,113 +3064,107 @@
       <c r="AG13">
         <v>2050</v>
       </c>
-      <c r="AH13">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>23</v>
       </c>
       <c r="B14"/>
-      <c r="C14">
-        <v>49996</v>
-      </c>
-      <c r="D14">
-        <v>48711.8</v>
-      </c>
-      <c r="E14">
-        <v>47597.7</v>
-      </c>
-      <c r="F14">
-        <v>46574.5</v>
-      </c>
-      <c r="G14">
-        <v>45651.8</v>
-      </c>
-      <c r="H14">
-        <v>44834.400000000001</v>
-      </c>
-      <c r="I14">
-        <v>44101.5</v>
-      </c>
-      <c r="J14">
-        <v>43427.7</v>
-      </c>
-      <c r="K14">
-        <v>42817.1</v>
-      </c>
-      <c r="L14">
-        <v>42254.3</v>
-      </c>
-      <c r="M14">
-        <v>41739.699999999997</v>
-      </c>
-      <c r="N14">
-        <v>41286.5</v>
-      </c>
-      <c r="O14">
-        <v>40889.599999999999</v>
-      </c>
-      <c r="P14">
-        <v>40537</v>
-      </c>
-      <c r="Q14">
-        <v>40226.199999999997</v>
-      </c>
-      <c r="R14">
-        <v>39954.300000000003</v>
-      </c>
-      <c r="S14">
-        <v>39717</v>
-      </c>
-      <c r="T14">
-        <v>39506.800000000003</v>
-      </c>
-      <c r="U14">
-        <v>39319.199999999997</v>
-      </c>
-      <c r="V14">
-        <v>39152.199999999997</v>
-      </c>
-      <c r="W14">
-        <v>39003.9</v>
-      </c>
-      <c r="X14">
-        <v>38872</v>
-      </c>
-      <c r="Y14">
-        <v>38753.5</v>
-      </c>
-      <c r="Z14">
-        <v>38646.6</v>
-      </c>
-      <c r="AA14">
-        <v>38549.699999999997</v>
-      </c>
-      <c r="AB14">
-        <v>38461.4</v>
-      </c>
-      <c r="AC14">
-        <v>38380.6</v>
-      </c>
-      <c r="AD14">
-        <v>38306.300000000003</v>
-      </c>
-      <c r="AE14">
-        <v>38237.699999999997</v>
-      </c>
-      <c r="AF14">
-        <v>38174.199999999997</v>
-      </c>
-      <c r="AG14">
-        <v>38115.1</v>
-      </c>
-      <c r="AH14">
-        <v>40174.6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="C14" s="19">
+        <v>51941</v>
+      </c>
+      <c r="D14" s="19">
+        <v>50597.9</v>
+      </c>
+      <c r="E14" s="19">
+        <v>49434.9</v>
+      </c>
+      <c r="F14" s="19">
+        <v>48369.8</v>
+      </c>
+      <c r="G14" s="19">
+        <v>47411</v>
+      </c>
+      <c r="H14" s="19">
+        <v>46562.1</v>
+      </c>
+      <c r="I14" s="19">
+        <v>45801.4</v>
+      </c>
+      <c r="J14" s="19">
+        <v>45102.3</v>
+      </c>
+      <c r="K14" s="19">
+        <v>44468.800000000003</v>
+      </c>
+      <c r="L14" s="19">
+        <v>43885.1</v>
+      </c>
+      <c r="M14" s="19">
+        <v>43351.5</v>
+      </c>
+      <c r="N14" s="19">
+        <v>42881.7</v>
+      </c>
+      <c r="O14" s="19">
+        <v>42470.3</v>
+      </c>
+      <c r="P14" s="19">
+        <v>42104.9</v>
+      </c>
+      <c r="Q14" s="19">
+        <v>41783.1</v>
+      </c>
+      <c r="R14" s="19">
+        <v>41501.5</v>
+      </c>
+      <c r="S14" s="19">
+        <v>41255.800000000003</v>
+      </c>
+      <c r="T14" s="19">
+        <v>41038.1</v>
+      </c>
+      <c r="U14" s="19">
+        <v>40844</v>
+      </c>
+      <c r="V14" s="19">
+        <v>40671</v>
+      </c>
+      <c r="W14" s="19">
+        <v>40517.5</v>
+      </c>
+      <c r="X14" s="19">
+        <v>40380.9</v>
+      </c>
+      <c r="Y14" s="19">
+        <v>40258.199999999997</v>
+      </c>
+      <c r="Z14" s="19">
+        <v>40147.4</v>
+      </c>
+      <c r="AA14" s="19">
+        <v>40047</v>
+      </c>
+      <c r="AB14" s="19">
+        <v>39955.5</v>
+      </c>
+      <c r="AC14" s="19">
+        <v>39871.800000000003</v>
+      </c>
+      <c r="AD14" s="19">
+        <v>39794.800000000003</v>
+      </c>
+      <c r="AE14" s="19">
+        <v>39723.699999999997</v>
+      </c>
+      <c r="AF14" s="19">
+        <v>39657.800000000003</v>
+      </c>
+      <c r="AG14" s="19">
+        <v>39596.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -3273,128 +3268,128 @@
     <row r="18" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="4">
-        <f t="shared" ref="A18:AF18" si="0">B11/C14</f>
-        <v>9.3080625079941276E-2</v>
+        <f t="shared" ref="B18:AF18" si="0">B11/C14</f>
+        <v>8.9595096965725415E-2</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="0"/>
-        <v>9.5534530267753312E-2</v>
+        <v>9.1973361176980586E-2</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="0"/>
-        <v>8.224893325394933E-2</v>
+        <v>7.9192231608468985E-2</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>7.6796345842659999E-2</v>
+        <v>7.3945962345285027E-2</v>
       </c>
       <c r="F18" s="4">
         <f t="shared" si="0"/>
-        <v>7.0566381391198543E-2</v>
+        <v>6.7947993714427404E-2</v>
       </c>
       <c r="G18" s="4">
         <f t="shared" si="0"/>
-        <v>6.793038014345798E-2</v>
+        <v>6.5409804014506495E-2</v>
       </c>
       <c r="H18" s="4">
         <f t="shared" si="0"/>
-        <v>6.9059279967888895E-2</v>
+        <v>6.6496173381247123E-2</v>
       </c>
       <c r="I18" s="4">
         <f t="shared" si="0"/>
-        <v>6.6266312664335247E-2</v>
+        <v>6.3805915585079948E-2</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" si="0"/>
-        <v>6.7211313855748106E-2</v>
+        <v>6.4714891035803787E-2</v>
       </c>
       <c r="K18" s="4">
         <f t="shared" si="0"/>
-        <v>6.5543406911182114E-2</v>
+        <v>6.310776957662538E-2</v>
       </c>
       <c r="L18" s="4">
         <f t="shared" si="0"/>
-        <v>5.8239568695682205E-2</v>
+        <v>5.607423331343013E-2</v>
       </c>
       <c r="M18" s="4">
         <f t="shared" si="0"/>
-        <v>5.4112048631594703E-2</v>
+        <v>5.2099079463461914E-2</v>
       </c>
       <c r="N18" s="4">
         <f t="shared" si="0"/>
-        <v>5.463729397764553E-2</v>
+        <v>5.2603751229172727E-2</v>
       </c>
       <c r="O18" s="4">
         <f t="shared" si="0"/>
-        <v>5.5112541525725499E-2</v>
+        <v>5.3060263670697105E-2</v>
       </c>
       <c r="P18" s="4">
         <f t="shared" si="0"/>
-        <v>5.5538357981323984E-2</v>
+        <v>5.3468916758888992E-2</v>
       </c>
       <c r="Q18" s="4">
         <f t="shared" si="0"/>
-        <v>5.5916311781919206E-2</v>
+        <v>5.3831719234927286E-2</v>
       </c>
       <c r="R18" s="4">
         <f t="shared" si="0"/>
-        <v>5.6250398968409866E-2</v>
+        <v>5.4152315452089997E-2</v>
       </c>
       <c r="S18" s="4">
         <f t="shared" si="0"/>
-        <v>5.6549685011905153E-2</v>
+        <v>5.4439584089622441E-2</v>
       </c>
       <c r="T18" s="4">
         <f t="shared" si="0"/>
-        <v>5.6404420200173847E-2</v>
+        <v>5.4298714100839182E-2</v>
       </c>
       <c r="U18" s="4">
         <f t="shared" si="0"/>
-        <v>5.6645007911041413E-2</v>
+        <v>5.4529681560194623E-2</v>
       </c>
       <c r="V18" s="4">
         <f t="shared" si="0"/>
-        <v>5.686038264723977E-2</v>
+        <v>5.4736266520261007E-2</v>
       </c>
       <c r="W18" s="4">
         <f t="shared" si="0"/>
-        <v>5.7053320609556375E-2</v>
+        <v>5.4921427673347435E-2</v>
       </c>
       <c r="X18" s="4">
         <f t="shared" si="0"/>
-        <v>5.7227777587435337E-2</v>
+        <v>5.5088818644019745E-2</v>
       </c>
       <c r="Y18" s="4">
         <f t="shared" si="0"/>
-        <v>5.7386074809547945E-2</v>
+        <v>5.5240854419829809E-2</v>
       </c>
       <c r="Z18" s="4">
         <f t="shared" si="0"/>
-        <v>5.7530322641542619E-2</v>
+        <v>5.5379346236538951E-2</v>
       </c>
       <c r="AA18" s="4">
         <f t="shared" si="0"/>
-        <v>5.7662401231745992E-2</v>
+        <v>5.5506167579799412E-2</v>
       </c>
       <c r="AB18" s="4">
         <f t="shared" si="0"/>
-        <v>5.7783793862906663E-2</v>
+        <v>5.5622687682388941E-2</v>
       </c>
       <c r="AC18" s="4">
         <f t="shared" si="0"/>
-        <v>5.7895872969581381E-2</v>
+        <v>5.5730313476501335E-2</v>
       </c>
       <c r="AD18" s="4">
         <f t="shared" si="0"/>
-        <v>5.7999740537079257E-2</v>
+        <v>5.5830063129433449E-2</v>
       </c>
       <c r="AE18" s="4">
         <f t="shared" si="0"/>
-        <v>5.8096218879103573E-2</v>
+        <v>5.5922836837511793E-2</v>
       </c>
       <c r="AF18" s="4">
         <f t="shared" si="0"/>
-        <v>5.8186300934135696E-2</v>
+        <v>5.600941191101929E-2</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.35">
@@ -3409,6 +3404,501 @@
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
       <c r="L30" s="4"/>
+    </row>
+    <row r="51" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="7"/>
+      <c r="R51" s="7"/>
+      <c r="S51" s="7"/>
+      <c r="T51" s="7"/>
+      <c r="U51" s="7"/>
+      <c r="V51" s="7"/>
+      <c r="W51" s="7"/>
+      <c r="X51" s="7"/>
+      <c r="Y51" s="7"/>
+      <c r="Z51" s="7"/>
+      <c r="AA51" s="7"/>
+      <c r="AB51" s="7"/>
+      <c r="AC51" s="7"/>
+      <c r="AD51" s="7"/>
+      <c r="AE51" s="7"/>
+      <c r="AF51" s="7"/>
+    </row>
+    <row r="54" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="7"/>
+      <c r="S54" s="7"/>
+      <c r="T54" s="7"/>
+      <c r="U54" s="7"/>
+      <c r="V54" s="7"/>
+      <c r="W54" s="7"/>
+      <c r="X54" s="7"/>
+      <c r="Y54" s="7"/>
+      <c r="Z54" s="7"/>
+      <c r="AA54" s="7"/>
+      <c r="AB54" s="7"/>
+      <c r="AC54" s="7"/>
+      <c r="AD54" s="7"/>
+      <c r="AE54" s="7"/>
+      <c r="AF54" s="7"/>
+    </row>
+    <row r="57" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="7"/>
+      <c r="P57" s="7"/>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="7"/>
+      <c r="S57" s="7"/>
+      <c r="T57" s="7"/>
+      <c r="U57" s="7"/>
+      <c r="V57" s="7"/>
+      <c r="W57" s="7"/>
+      <c r="X57" s="7"/>
+      <c r="Y57" s="7"/>
+      <c r="Z57" s="7"/>
+      <c r="AA57" s="7"/>
+      <c r="AB57" s="7"/>
+      <c r="AC57" s="7"/>
+      <c r="AD57" s="7"/>
+      <c r="AE57" s="7"/>
+      <c r="AF57" s="7"/>
+    </row>
+    <row r="58" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="7"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
+      <c r="N58" s="7"/>
+      <c r="O58" s="7"/>
+      <c r="P58" s="7"/>
+      <c r="Q58" s="7"/>
+      <c r="R58" s="7"/>
+      <c r="S58" s="7"/>
+      <c r="T58" s="7"/>
+      <c r="U58" s="7"/>
+      <c r="V58" s="7"/>
+      <c r="W58" s="7"/>
+      <c r="X58" s="7"/>
+      <c r="Y58" s="7"/>
+      <c r="Z58" s="7"/>
+      <c r="AA58" s="7"/>
+      <c r="AB58" s="7"/>
+      <c r="AC58" s="7"/>
+      <c r="AD58" s="7"/>
+      <c r="AE58" s="7"/>
+      <c r="AF58" s="7"/>
+    </row>
+    <row r="61" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
+      <c r="L61" s="7"/>
+      <c r="M61" s="7"/>
+      <c r="N61" s="7"/>
+      <c r="O61" s="7"/>
+      <c r="P61" s="7"/>
+      <c r="Q61" s="7"/>
+      <c r="R61" s="7"/>
+      <c r="S61" s="7"/>
+      <c r="T61" s="7"/>
+      <c r="U61" s="7"/>
+      <c r="V61" s="7"/>
+      <c r="W61" s="7"/>
+      <c r="X61" s="7"/>
+      <c r="Y61" s="7"/>
+      <c r="Z61" s="7"/>
+      <c r="AA61" s="7"/>
+      <c r="AB61" s="7"/>
+      <c r="AC61" s="7"/>
+      <c r="AD61" s="7"/>
+      <c r="AE61" s="7"/>
+      <c r="AF61" s="7"/>
+    </row>
+    <row r="64" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="7"/>
+      <c r="P64" s="7"/>
+      <c r="Q64" s="7"/>
+      <c r="R64" s="7"/>
+      <c r="S64" s="7"/>
+      <c r="T64" s="7"/>
+      <c r="U64" s="7"/>
+      <c r="V64" s="7"/>
+      <c r="W64" s="7"/>
+      <c r="X64" s="7"/>
+      <c r="Y64" s="7"/>
+      <c r="Z64" s="7"/>
+      <c r="AA64" s="7"/>
+      <c r="AB64" s="7"/>
+      <c r="AC64" s="7"/>
+      <c r="AD64" s="7"/>
+      <c r="AE64" s="7"/>
+      <c r="AF64" s="7"/>
+    </row>
+    <row r="65" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="7"/>
+      <c r="P65" s="7"/>
+      <c r="Q65" s="7"/>
+      <c r="R65" s="7"/>
+      <c r="S65" s="7"/>
+      <c r="T65" s="7"/>
+      <c r="U65" s="7"/>
+      <c r="V65" s="7"/>
+      <c r="W65" s="7"/>
+      <c r="X65" s="7"/>
+      <c r="Y65" s="7"/>
+      <c r="Z65" s="7"/>
+      <c r="AA65" s="7"/>
+      <c r="AB65" s="7"/>
+      <c r="AC65" s="7"/>
+      <c r="AD65" s="7"/>
+      <c r="AE65" s="7"/>
+      <c r="AF65" s="7"/>
+    </row>
+    <row r="68" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
+      <c r="L68" s="7"/>
+      <c r="M68" s="7"/>
+      <c r="N68" s="7"/>
+      <c r="O68" s="7"/>
+      <c r="P68" s="7"/>
+      <c r="Q68" s="7"/>
+      <c r="R68" s="7"/>
+      <c r="S68" s="7"/>
+      <c r="T68" s="7"/>
+      <c r="U68" s="7"/>
+      <c r="V68" s="7"/>
+      <c r="W68" s="7"/>
+      <c r="X68" s="7"/>
+      <c r="Y68" s="7"/>
+      <c r="Z68" s="7"/>
+      <c r="AA68" s="7"/>
+      <c r="AB68" s="7"/>
+      <c r="AC68" s="7"/>
+      <c r="AD68" s="7"/>
+      <c r="AE68" s="7"/>
+      <c r="AF68" s="7"/>
+    </row>
+    <row r="71" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
+      <c r="N71" s="7"/>
+      <c r="O71" s="7"/>
+      <c r="P71" s="7"/>
+      <c r="Q71" s="7"/>
+      <c r="R71" s="7"/>
+      <c r="S71" s="7"/>
+      <c r="T71" s="7"/>
+      <c r="U71" s="7"/>
+      <c r="V71" s="7"/>
+      <c r="W71" s="7"/>
+      <c r="X71" s="7"/>
+      <c r="Y71" s="7"/>
+      <c r="Z71" s="7"/>
+      <c r="AA71" s="7"/>
+      <c r="AB71" s="7"/>
+      <c r="AC71" s="7"/>
+      <c r="AD71" s="7"/>
+      <c r="AE71" s="7"/>
+      <c r="AF71" s="7"/>
+    </row>
+    <row r="72" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+      <c r="I72" s="7"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="7"/>
+      <c r="L72" s="7"/>
+      <c r="M72" s="7"/>
+      <c r="N72" s="7"/>
+      <c r="O72" s="7"/>
+      <c r="P72" s="7"/>
+      <c r="Q72" s="7"/>
+      <c r="R72" s="7"/>
+      <c r="S72" s="7"/>
+      <c r="T72" s="7"/>
+      <c r="U72" s="7"/>
+      <c r="V72" s="7"/>
+      <c r="W72" s="7"/>
+      <c r="X72" s="7"/>
+      <c r="Y72" s="7"/>
+      <c r="Z72" s="7"/>
+      <c r="AA72" s="7"/>
+      <c r="AB72" s="7"/>
+      <c r="AC72" s="7"/>
+      <c r="AD72" s="7"/>
+      <c r="AE72" s="7"/>
+      <c r="AF72" s="7"/>
+    </row>
+    <row r="75" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="7"/>
+      <c r="M75" s="7"/>
+      <c r="N75" s="7"/>
+      <c r="O75" s="7"/>
+      <c r="P75" s="7"/>
+      <c r="Q75" s="7"/>
+      <c r="R75" s="7"/>
+      <c r="S75" s="7"/>
+      <c r="T75" s="7"/>
+      <c r="U75" s="7"/>
+      <c r="V75" s="7"/>
+      <c r="W75" s="7"/>
+      <c r="X75" s="7"/>
+      <c r="Y75" s="7"/>
+      <c r="Z75" s="7"/>
+      <c r="AA75" s="7"/>
+      <c r="AB75" s="7"/>
+      <c r="AC75" s="7"/>
+      <c r="AD75" s="7"/>
+      <c r="AE75" s="7"/>
+      <c r="AF75" s="7"/>
+    </row>
+    <row r="78" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="I78" s="7"/>
+      <c r="J78" s="7"/>
+      <c r="K78" s="7"/>
+      <c r="L78" s="7"/>
+      <c r="M78" s="7"/>
+      <c r="N78" s="7"/>
+      <c r="O78" s="7"/>
+      <c r="P78" s="7"/>
+      <c r="Q78" s="7"/>
+      <c r="R78" s="7"/>
+      <c r="S78" s="7"/>
+      <c r="T78" s="7"/>
+      <c r="U78" s="7"/>
+      <c r="V78" s="7"/>
+      <c r="W78" s="7"/>
+      <c r="X78" s="7"/>
+      <c r="Y78" s="7"/>
+      <c r="Z78" s="7"/>
+      <c r="AA78" s="7"/>
+      <c r="AB78" s="7"/>
+      <c r="AC78" s="7"/>
+      <c r="AD78" s="7"/>
+      <c r="AE78" s="7"/>
+      <c r="AF78" s="7"/>
+    </row>
+    <row r="86" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7"/>
+      <c r="I86" s="7"/>
+      <c r="J86" s="7"/>
+      <c r="K86" s="7"/>
+      <c r="L86" s="7"/>
+      <c r="M86" s="7"/>
+      <c r="N86" s="7"/>
+      <c r="O86" s="7"/>
+      <c r="P86" s="7"/>
+      <c r="Q86" s="7"/>
+      <c r="R86" s="7"/>
+      <c r="S86" s="7"/>
+      <c r="T86" s="7"/>
+      <c r="U86" s="7"/>
+      <c r="V86" s="7"/>
+      <c r="W86" s="7"/>
+      <c r="X86" s="7"/>
+      <c r="Y86" s="7"/>
+      <c r="Z86" s="7"/>
+      <c r="AA86" s="7"/>
+      <c r="AB86" s="7"/>
+      <c r="AC86" s="7"/>
+      <c r="AD86" s="7"/>
+      <c r="AE86" s="7"/>
+      <c r="AF86" s="7"/>
+    </row>
+    <row r="89" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7"/>
+      <c r="H89" s="7"/>
+      <c r="I89" s="7"/>
+      <c r="J89" s="7"/>
+      <c r="K89" s="7"/>
+      <c r="L89" s="7"/>
+      <c r="M89" s="7"/>
+      <c r="N89" s="7"/>
+      <c r="O89" s="7"/>
+      <c r="P89" s="7"/>
+      <c r="Q89" s="7"/>
+      <c r="R89" s="7"/>
+      <c r="S89" s="7"/>
+      <c r="T89" s="7"/>
+      <c r="U89" s="7"/>
+      <c r="V89" s="7"/>
+      <c r="W89" s="7"/>
+      <c r="X89" s="7"/>
+      <c r="Y89" s="7"/>
+      <c r="Z89" s="7"/>
+      <c r="AA89" s="7"/>
+      <c r="AB89" s="7"/>
+      <c r="AC89" s="7"/>
+      <c r="AD89" s="7"/>
+      <c r="AE89" s="7"/>
+      <c r="AF89" s="7"/>
+    </row>
+    <row r="92" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
+      <c r="F92" s="7"/>
+      <c r="G92" s="7"/>
+      <c r="H92" s="7"/>
+      <c r="I92" s="7"/>
+      <c r="J92" s="7"/>
+      <c r="K92" s="7"/>
+      <c r="L92" s="7"/>
+      <c r="M92" s="7"/>
+      <c r="N92" s="7"/>
+      <c r="O92" s="7"/>
+      <c r="P92" s="7"/>
+      <c r="Q92" s="7"/>
+      <c r="R92" s="7"/>
+      <c r="S92" s="7"/>
+      <c r="T92" s="7"/>
+      <c r="U92" s="7"/>
+      <c r="V92" s="7"/>
+      <c r="W92" s="7"/>
+      <c r="X92" s="7"/>
+      <c r="Y92" s="7"/>
+      <c r="Z92" s="7"/>
+      <c r="AA92" s="7"/>
+      <c r="AB92" s="7"/>
+      <c r="AC92" s="7"/>
+      <c r="AD92" s="7"/>
+      <c r="AE92" s="7"/>
+      <c r="AF92" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13260,7 +13750,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>130</v>
       </c>
       <c r="B1" t="s">
@@ -13274,7 +13764,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="19"/>
+      <c r="A2" s="21"/>
       <c r="B2" t="s">
         <v>134</v>
       </c>
@@ -13286,7 +13776,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="19"/>
+      <c r="A3" s="21"/>
       <c r="C3">
         <v>200000</v>
       </c>
@@ -13295,7 +13785,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
+      <c r="A4" s="21"/>
       <c r="D4">
         <v>200000</v>
       </c>
@@ -13694,127 +14184,127 @@
       </c>
       <c r="F2" s="18">
         <f>Data!B18</f>
-        <v>9.3080625079941276E-2</v>
+        <v>8.9595096965725415E-2</v>
       </c>
       <c r="G2" s="18">
         <f>Data!C18</f>
-        <v>9.5534530267753312E-2</v>
+        <v>9.1973361176980586E-2</v>
       </c>
       <c r="H2" s="18">
         <f>Data!D18</f>
-        <v>8.224893325394933E-2</v>
+        <v>7.9192231608468985E-2</v>
       </c>
       <c r="I2" s="18">
         <f>Data!E18</f>
-        <v>7.6796345842659999E-2</v>
+        <v>7.3945962345285027E-2</v>
       </c>
       <c r="J2" s="18">
         <f>Data!F18</f>
-        <v>7.0566381391198543E-2</v>
+        <v>6.7947993714427404E-2</v>
       </c>
       <c r="K2" s="18">
         <f>Data!G18</f>
-        <v>6.793038014345798E-2</v>
+        <v>6.5409804014506495E-2</v>
       </c>
       <c r="L2" s="18">
         <f>Data!H18</f>
-        <v>6.9059279967888895E-2</v>
+        <v>6.6496173381247123E-2</v>
       </c>
       <c r="M2" s="18">
         <f>Data!I18</f>
-        <v>6.6266312664335247E-2</v>
+        <v>6.3805915585079948E-2</v>
       </c>
       <c r="N2" s="18">
         <f>Data!J18</f>
-        <v>6.7211313855748106E-2</v>
+        <v>6.4714891035803787E-2</v>
       </c>
       <c r="O2" s="18">
         <f>Data!K18</f>
-        <v>6.5543406911182114E-2</v>
+        <v>6.310776957662538E-2</v>
       </c>
       <c r="P2" s="18">
         <f>Data!L18</f>
-        <v>5.8239568695682205E-2</v>
+        <v>5.607423331343013E-2</v>
       </c>
       <c r="Q2" s="18">
         <f>Data!M18</f>
-        <v>5.4112048631594703E-2</v>
+        <v>5.2099079463461914E-2</v>
       </c>
       <c r="R2" s="18">
         <f>Data!N18</f>
-        <v>5.463729397764553E-2</v>
+        <v>5.2603751229172727E-2</v>
       </c>
       <c r="S2" s="18">
         <f>Data!O18</f>
-        <v>5.5112541525725499E-2</v>
+        <v>5.3060263670697105E-2</v>
       </c>
       <c r="T2" s="18">
         <f>Data!P18</f>
-        <v>5.5538357981323984E-2</v>
+        <v>5.3468916758888992E-2</v>
       </c>
       <c r="U2" s="18">
         <f>Data!Q18</f>
-        <v>5.5916311781919206E-2</v>
+        <v>5.3831719234927286E-2</v>
       </c>
       <c r="V2" s="18">
         <f>Data!R18</f>
-        <v>5.6250398968409866E-2</v>
+        <v>5.4152315452089997E-2</v>
       </c>
       <c r="W2" s="18">
         <f>Data!S18</f>
-        <v>5.6549685011905153E-2</v>
+        <v>5.4439584089622441E-2</v>
       </c>
       <c r="X2" s="18">
         <f>Data!T18</f>
-        <v>5.6404420200173847E-2</v>
+        <v>5.4298714100839182E-2</v>
       </c>
       <c r="Y2" s="18">
         <f>Data!U18</f>
-        <v>5.6645007911041413E-2</v>
+        <v>5.4529681560194623E-2</v>
       </c>
       <c r="Z2" s="18">
         <f>Data!V18</f>
-        <v>5.686038264723977E-2</v>
+        <v>5.4736266520261007E-2</v>
       </c>
       <c r="AA2" s="18">
         <f>Data!W18</f>
-        <v>5.7053320609556375E-2</v>
+        <v>5.4921427673347435E-2</v>
       </c>
       <c r="AB2" s="18">
         <f>Data!X18</f>
-        <v>5.7227777587435337E-2</v>
+        <v>5.5088818644019745E-2</v>
       </c>
       <c r="AC2" s="18">
         <f>Data!Y18</f>
-        <v>5.7386074809547945E-2</v>
+        <v>5.5240854419829809E-2</v>
       </c>
       <c r="AD2" s="18">
         <f>Data!Z18</f>
-        <v>5.7530322641542619E-2</v>
+        <v>5.5379346236538951E-2</v>
       </c>
       <c r="AE2" s="18">
         <f>Data!AA18</f>
-        <v>5.7662401231745992E-2</v>
+        <v>5.5506167579799412E-2</v>
       </c>
       <c r="AF2" s="18">
         <f>Data!AB18</f>
-        <v>5.7783793862906663E-2</v>
+        <v>5.5622687682388941E-2</v>
       </c>
       <c r="AG2" s="18">
         <f>Data!AC18</f>
-        <v>5.7895872969581381E-2</v>
+        <v>5.5730313476501335E-2</v>
       </c>
       <c r="AH2" s="18">
         <f>Data!AD18</f>
-        <v>5.7999740537079257E-2</v>
+        <v>5.5830063129433449E-2</v>
       </c>
       <c r="AI2" s="18">
         <f>Data!AE18</f>
-        <v>5.8096218879103573E-2</v>
+        <v>5.5922836837511793E-2</v>
       </c>
       <c r="AJ2" s="18">
         <f>Data!AF18</f>
-        <v>5.8186300934135696E-2</v>
+        <v>5.600941191101929E-2</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">

</xml_diff>